<commit_message>
Userstories aktualisiert und die erste Userstorie in Tasks zerlegt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275AC513-2703-4837-A098-E1ABE5FD9302}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E09C5E0-9B1A-4AF2-911E-3ACA36E667D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Userstories</t>
   </si>
@@ -148,6 +148,39 @@
   </si>
   <si>
     <t>Als Admin soll man die Möglichkeit haben das Layout der Seite zu ändern</t>
+  </si>
+  <si>
+    <t>Als Benutzer soll man ein angemessenes Layout sehen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als Benutzer soll man seine Profil bearbbeiten können </t>
+  </si>
+  <si>
+    <t>1. Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als registrierter Benutzer soll man mit anderen kommunizieren könnenn und Posts verfassen können </t>
+  </si>
+  <si>
+    <t>Layout für das Anmeldefenster erzeugen</t>
+  </si>
+  <si>
+    <t>2. Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layout für die Hauptseite erzeugen </t>
+  </si>
+  <si>
+    <t>Verantwortlicher</t>
+  </si>
+  <si>
+    <t>Manuel</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Endzeitpunkt</t>
   </si>
 </sst>
 </file>
@@ -201,8 +234,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -210,6 +246,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -492,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,77 +543,77 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="O6" s="1" t="s">
+      <c r="D6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="O6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="O7" t="s">
         <v>3</v>
       </c>
@@ -585,15 +625,15 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
       <c r="O8" t="s">
         <v>2</v>
       </c>
@@ -605,15 +645,15 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
       <c r="O9" t="s">
         <v>4</v>
       </c>
@@ -773,89 +813,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353FBFB2-16BE-4644-9382-36A3ABDFA74F}">
   <dimension ref="C3:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -873,14 +914,172 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="A1"/>
+  <dimension ref="B4:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="6">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="6">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C18:I18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UserStories auf aktuellen Stand aktualisiert
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E09C5E0-9B1A-4AF2-911E-3ACA36E667D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE35AD5-1BF3-45FC-8896-4A7360786981}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>Userstories</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>Endzeitpunkt</t>
+  </si>
+  <si>
+    <t>3. Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layout für die Registrierung erzeugen </t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>in Arbeit</t>
   </si>
 </sst>
 </file>
@@ -239,17 +251,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -533,87 +545,87 @@
   <dimension ref="C3:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D4" sqref="D4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="O6" s="2" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="O6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
       <c r="O7" t="s">
         <v>3</v>
       </c>
@@ -621,19 +633,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
       <c r="O8" t="s">
         <v>2</v>
       </c>
@@ -641,19 +653,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
       <c r="O9" t="s">
         <v>4</v>
       </c>
@@ -661,7 +673,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O10" t="s">
         <v>5</v>
       </c>
@@ -669,7 +681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O11" t="s">
         <v>6</v>
       </c>
@@ -677,7 +689,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O12" t="s">
         <v>7</v>
       </c>
@@ -685,7 +697,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
         <v>8</v>
       </c>
@@ -693,7 +705,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O14" t="s">
         <v>9</v>
       </c>
@@ -701,7 +713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O15" t="s">
         <v>10</v>
       </c>
@@ -709,7 +721,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O16" t="s">
         <v>11</v>
       </c>
@@ -717,7 +729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -725,7 +737,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O18" t="s">
         <v>13</v>
       </c>
@@ -733,7 +745,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O19" t="s">
         <v>14</v>
       </c>
@@ -741,7 +753,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O20" t="s">
         <v>15</v>
       </c>
@@ -749,7 +761,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O21" t="s">
         <v>16</v>
       </c>
@@ -757,7 +769,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O22" t="s">
         <v>17</v>
       </c>
@@ -765,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O23" t="s">
         <v>18</v>
       </c>
@@ -773,22 +785,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O27" t="s">
         <v>22</v>
       </c>
@@ -817,86 +829,86 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="3" t="s">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="3" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="3" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="3" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -914,68 +926,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:K20"/>
+  <dimension ref="B4:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="14.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" t="s">
         <v>49</v>
       </c>
       <c r="K6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>44</v>
       </c>
@@ -985,87 +1001,101 @@
       <c r="J8" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="3">
         <v>43515</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="3">
         <v>43515</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C14" s="3" t="s">
+      <c r="L9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C15" s="3" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C16" s="3" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="3" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="3" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Userstories erneuert und die Verwendung von Materialize ermöglicht. Ebenso noch ein grundlegendes Design für die Anmeldeseite hinzugefügt.
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE35AD5-1BF3-45FC-8896-4A7360786981}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D823DB2-EA46-40F7-8C5E-F8AD648958FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Userstories</t>
   </si>
@@ -162,9 +162,6 @@
     <t xml:space="preserve">Als registrierter Benutzer soll man mit anderen kommunizieren könnenn und Posts verfassen können </t>
   </si>
   <si>
-    <t>Layout für das Anmeldefenster erzeugen</t>
-  </si>
-  <si>
     <t>2. Task</t>
   </si>
   <si>
@@ -183,16 +180,16 @@
     <t>Endzeitpunkt</t>
   </si>
   <si>
-    <t>3. Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layout für die Registrierung erzeugen </t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>in Arbeit</t>
+  </si>
+  <si>
+    <t>Layout für das Anmeldefenster und Registrierungsfenster erzeugen</t>
+  </si>
+  <si>
+    <t>19.02.209</t>
   </si>
 </sst>
 </file>
@@ -548,13 +545,13 @@
       <selection activeCell="D4" sqref="D4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -566,7 +563,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -580,7 +577,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -594,7 +591,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -613,7 +610,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -633,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -653,7 +650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -673,7 +670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O10" t="s">
         <v>5</v>
       </c>
@@ -681,7 +678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O11" t="s">
         <v>6</v>
       </c>
@@ -689,7 +686,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O12" t="s">
         <v>7</v>
       </c>
@@ -697,7 +694,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O13" t="s">
         <v>8</v>
       </c>
@@ -705,7 +702,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O14" t="s">
         <v>9</v>
       </c>
@@ -713,7 +710,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O15" t="s">
         <v>10</v>
       </c>
@@ -721,7 +718,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O16" t="s">
         <v>11</v>
       </c>
@@ -729,7 +726,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -737,7 +734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O18" t="s">
         <v>13</v>
       </c>
@@ -745,7 +742,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O19" t="s">
         <v>14</v>
       </c>
@@ -753,7 +750,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O20" t="s">
         <v>15</v>
       </c>
@@ -761,7 +758,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O21" t="s">
         <v>16</v>
       </c>
@@ -769,7 +766,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O22" t="s">
         <v>17</v>
       </c>
@@ -777,7 +774,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O23" t="s">
         <v>18</v>
       </c>
@@ -785,22 +782,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O27" t="s">
         <v>22</v>
       </c>
@@ -829,9 +826,9 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -843,7 +840,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
@@ -855,7 +852,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
@@ -866,7 +863,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
@@ -877,7 +874,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
         <v>41</v>
       </c>
@@ -888,7 +885,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>39</v>
       </c>
@@ -899,7 +896,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
         <v>40</v>
       </c>
@@ -929,16 +926,16 @@
   <dimension ref="B4:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -948,7 +945,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -957,7 +954,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
@@ -968,16 +965,16 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" t="s">
         <v>52</v>
       </c>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -991,49 +988,41 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K8" s="3">
         <v>43515</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
       <c r="J9" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="3">
-        <v>43515</v>
+        <v>49</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="L9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
         <v>53</v>
       </c>
-      <c r="D10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
         <v>1</v>
       </c>
@@ -1044,7 +1033,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1055,7 +1044,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
         <v>41</v>
       </c>
@@ -1066,7 +1055,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" s="4" t="s">
         <v>39</v>
       </c>
@@ -1077,7 +1066,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
@@ -1088,7 +1077,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>

</xml_diff>

<commit_message>
Userstories sind erneuert; weitere Aufgaben bis zum 19.02.2019 hinzugefügt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AE2FAE-2DC4-4E56-9DB4-450D5FCC98AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13831F93-C651-4BFF-B846-87014CDF1B03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Userstories</t>
   </si>
@@ -192,7 +192,25 @@
     <t>Status</t>
   </si>
   <si>
-    <t>in Arbeit</t>
+    <t>abgeschlossen</t>
+  </si>
+  <si>
+    <t>Datenbank erzeugen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datenbankmethoden schreiben </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Task </t>
+  </si>
+  <si>
+    <t>Die Methode zum Registrieren schreiben</t>
+  </si>
+  <si>
+    <t>4. Task</t>
+  </si>
+  <si>
+    <t>Die Methode zum Anmelden schreiben</t>
   </si>
 </sst>
 </file>
@@ -246,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -262,6 +280,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -548,13 +567,13 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -566,7 +585,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -580,7 +599,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -594,7 +613,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -613,7 +632,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -633,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -653,7 +672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -673,7 +692,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O10" t="s">
         <v>5</v>
       </c>
@@ -681,7 +700,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O11" t="s">
         <v>6</v>
       </c>
@@ -689,7 +708,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O12" t="s">
         <v>7</v>
       </c>
@@ -697,7 +716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O13" t="s">
         <v>8</v>
       </c>
@@ -705,7 +724,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O14" t="s">
         <v>9</v>
       </c>
@@ -713,7 +732,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O15" t="s">
         <v>10</v>
       </c>
@@ -721,7 +740,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
       <c r="O16" t="s">
         <v>11</v>
       </c>
@@ -729,7 +748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -737,7 +756,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O18" t="s">
         <v>13</v>
       </c>
@@ -745,7 +764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O19" t="s">
         <v>14</v>
       </c>
@@ -753,7 +772,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O20" t="s">
         <v>15</v>
       </c>
@@ -761,7 +780,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O21" t="s">
         <v>16</v>
       </c>
@@ -769,7 +788,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O22" t="s">
         <v>17</v>
       </c>
@@ -777,7 +796,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O23" t="s">
         <v>18</v>
       </c>
@@ -785,22 +804,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="15:16" x14ac:dyDescent="0.3">
       <c r="O27" t="s">
         <v>22</v>
       </c>
@@ -829,9 +848,9 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -843,7 +862,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
@@ -855,7 +874,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
@@ -866,7 +885,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
@@ -877,7 +896,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
         <v>41</v>
       </c>
@@ -888,7 +907,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
         <v>39</v>
       </c>
@@ -899,7 +918,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
         <v>40</v>
       </c>
@@ -926,19 +945,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:L20"/>
+  <dimension ref="B4:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -948,7 +967,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -957,7 +976,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
@@ -977,7 +996,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -991,7 +1010,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>44</v>
       </c>
@@ -1008,7 +1027,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>47</v>
       </c>
@@ -1016,7 +1035,7 @@
         <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K9" s="3">
         <v>43515</v>
@@ -1025,70 +1044,139 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>53</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+      <c r="J10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="3">
+        <v>43515</v>
+      </c>
+      <c r="L10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="3">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="3">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="3">
+        <v>43515</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="3">
+        <v>43515</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="L18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="L19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1102,13 +1190,13 @@
     <mergeCell ref="D20:J20"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C14:I14"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="L16:R16"/>
+    <mergeCell ref="L17:R17"/>
+    <mergeCell ref="L18:R18"/>
+    <mergeCell ref="L19:R19"/>
+    <mergeCell ref="C13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Alle Layouts auf Mobile- (Responsive-) Design optimiert
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13831F93-C651-4BFF-B846-87014CDF1B03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513BC75A-E3BF-4EA4-8DE3-8E9592B62915}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>Userstories</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>Die Methode zum Anmelden schreiben</t>
+  </si>
+  <si>
+    <t>in Bearbeitung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als registrierter Benutzer soll man sein Profil bearbbeiten können </t>
+  </si>
+  <si>
+    <t>alle Layouts für mobile Geräte optimieren</t>
   </si>
 </sst>
 </file>
@@ -264,13 +273,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -280,7 +298,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -567,84 +584,84 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="O6" s="5" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="O6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
       <c r="O7" t="s">
         <v>3</v>
       </c>
@@ -652,19 +669,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
       <c r="O8" t="s">
         <v>2</v>
       </c>
@@ -672,19 +689,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
       <c r="O9" t="s">
         <v>4</v>
       </c>
@@ -692,7 +709,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O10" t="s">
         <v>5</v>
       </c>
@@ -700,7 +717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O11" t="s">
         <v>6</v>
       </c>
@@ -708,7 +725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O12" t="s">
         <v>7</v>
       </c>
@@ -716,7 +733,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
         <v>8</v>
       </c>
@@ -724,7 +741,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O14" t="s">
         <v>9</v>
       </c>
@@ -732,7 +749,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O15" t="s">
         <v>10</v>
       </c>
@@ -740,7 +757,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="O16" t="s">
         <v>11</v>
       </c>
@@ -748,7 +765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -756,7 +773,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O18" t="s">
         <v>13</v>
       </c>
@@ -764,7 +781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O19" t="s">
         <v>14</v>
       </c>
@@ -772,7 +789,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O20" t="s">
         <v>15</v>
       </c>
@@ -780,7 +797,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O21" t="s">
         <v>16</v>
       </c>
@@ -788,7 +805,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O22" t="s">
         <v>17</v>
       </c>
@@ -796,7 +813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O23" t="s">
         <v>18</v>
       </c>
@@ -804,22 +821,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O27" t="s">
         <v>22</v>
       </c>
@@ -848,86 +865,86 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="4" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="4" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="4" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -945,184 +962,201 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R20"/>
+  <dimension ref="B4:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="D5" sqref="D5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>44</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="6">
         <v>43515</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>54</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="6">
         <v>43515</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>53</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="6">
         <v>43515</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="6">
+        <v>43515</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" t="s">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K15" s="6">
         <v>43515</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+      <c r="L15" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>58</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K16" s="6">
         <v>43515</v>
       </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" s="3">
-        <v>43515</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>28</v>
+      <c r="L16" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -1131,21 +1165,21 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17" s="6">
         <v>43515</v>
       </c>
-      <c r="L17" s="4" t="s">
-        <v>41</v>
+      <c r="L17" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -1154,9 +1188,21 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L18" s="4" t="s">
-        <v>39</v>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="6">
+        <v>43515</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -1165,10 +1211,8 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L19" s="4" t="s">
-        <v>40</v>
-      </c>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="J19" s="3"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1176,27 +1220,71 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="L23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="L24" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="L25" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="L26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="D20:J20"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
-    <mergeCell ref="L16:R16"/>
-    <mergeCell ref="L17:R17"/>
-    <mergeCell ref="L18:R18"/>
-    <mergeCell ref="L19:R19"/>
-    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="L23:R23"/>
+    <mergeCell ref="L24:R24"/>
+    <mergeCell ref="L25:R25"/>
+    <mergeCell ref="L26:R26"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="D20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Registrierung getestet und die Loginmethode erstellt, diese ist noch nicht fertig
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CA426A-40C7-451B-8EBD-F34406F85464}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F3050F-EB6F-414B-9444-11DB17CEF552}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
   <si>
     <t>Userstories</t>
   </si>
@@ -144,9 +144,6 @@
     <t xml:space="preserve">Als registrierter Benutzer soll man seine Profil bearbbeiten können </t>
   </si>
   <si>
-    <t xml:space="preserve">Als registrierter Benutzer soll man mit anderen kommunizieren können verfassen können </t>
-  </si>
-  <si>
     <t>Als Admin soll man die Möglichkeit haben das Layout der Seite zu ändern</t>
   </si>
   <si>
@@ -217,6 +214,33 @@
   </si>
   <si>
     <t>Der Benutzer soll eine Fehlermeldung bekommen wenn der Benutzername schon vergeben ist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Task </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Daten sollen bei der Registreierung überprüft werden </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als registrierter Benutzer soll man mit anderen kommunizieren können und Beiträge verfassen können </t>
+  </si>
+  <si>
+    <t>7. Task</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll die im Task 6 erzeugten Fehlermeldung in schöner Form angezeigt bekommen</t>
+  </si>
+  <si>
+    <t>Als Benutzer soll man sich mit einfachen Buttons durch die komplette Webseite klicken können</t>
+  </si>
+  <si>
+    <t>Als Benutzer soll man sich mit einfachen Buttons durch die komplette Seite klicken können</t>
+  </si>
+  <si>
+    <t>in Arbeit</t>
+  </si>
+  <si>
+    <t>responsive Design bei allen Layouts</t>
   </si>
 </sst>
 </file>
@@ -570,7 +594,7 @@
   <dimension ref="C3:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -624,7 +648,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -683,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -699,6 +723,12 @@
       </c>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
       <c r="O10" t="s">
         <v>5</v>
       </c>
@@ -848,10 +878,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353FBFB2-16BE-4644-9382-36A3ABDFA74F}">
-  <dimension ref="C3:J9"/>
+  <dimension ref="C3:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,7 +900,7 @@
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -892,19 +922,13 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -915,7 +939,7 @@
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -926,7 +950,7 @@
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -935,15 +959,26 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C8:I8"/>
     <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C10:I10"/>
     <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -953,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
   <dimension ref="B4:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,13 +1028,13 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -1007,7 +1042,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1018,53 +1053,70 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L8" s="3">
         <v>43515</v>
       </c>
       <c r="M8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L9" s="3">
         <v>43515</v>
       </c>
       <c r="M9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L10" s="3">
         <v>43515</v>
       </c>
       <c r="M10" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="3">
+        <v>43515</v>
+      </c>
+      <c r="M11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
@@ -1083,10 +1135,10 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1094,70 +1146,104 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="K14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L14" s="3">
         <v>43515</v>
       </c>
       <c r="M14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L15" s="3">
         <v>43515</v>
       </c>
       <c r="M15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
         <v>59</v>
       </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
       <c r="K16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L16" s="3">
         <v>43515</v>
       </c>
+      <c r="M16" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="17" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
         <v>61</v>
       </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
       <c r="K17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L17" s="3">
-        <v>43515</v>
+        <v>43522</v>
+      </c>
+      <c r="M17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
+      <c r="K18" t="s">
+        <v>49</v>
+      </c>
+      <c r="L18" s="3">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
         <v>64</v>
       </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="3">
+        <v>43515</v>
+      </c>
+      <c r="M19" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="D20" s="5"/>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1166,9 +1252,7 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L21" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -1177,9 +1261,7 @@
       <c r="R21" s="5"/>
     </row>
     <row r="22" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L22" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
@@ -1188,9 +1270,7 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L23" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -1199,9 +1279,7 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L24" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
@@ -1223,5 +1301,6 @@
     <mergeCell ref="D20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fehler beim Login behoben und ebenso noch eine Methode zum überprüfen ob ein Benutzername schon verwendet wird
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F3050F-EB6F-414B-9444-11DB17CEF552}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A60C792-0A89-4A4C-A86A-5E634BB57834}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>Userstories</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>responsive Design bei allen Layouts</t>
+  </si>
+  <si>
+    <t>In Arbeit</t>
   </si>
 </sst>
 </file>
@@ -989,7 +992,7 @@
   <dimension ref="B4:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,10 +1116,10 @@
         <v>49</v>
       </c>
       <c r="L11" s="3">
-        <v>43515</v>
+        <v>43517</v>
       </c>
       <c r="M11" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
@@ -1203,7 +1206,7 @@
         <v>43522</v>
       </c>
       <c r="M17" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="3:18" x14ac:dyDescent="0.3">
@@ -1214,10 +1217,13 @@
         <v>63</v>
       </c>
       <c r="K18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L18" s="3">
         <v>43522</v>
+      </c>
+      <c r="M18" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Die Registrierung erweitert und die Login fertiggestellt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A60C792-0A89-4A4C-A86A-5E634BB57834}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F85BF5-B319-4AE4-BAD2-0F1AFA467A2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
   <si>
     <t>Userstories</t>
   </si>
@@ -243,7 +243,10 @@
     <t>responsive Design bei allen Layouts</t>
   </si>
   <si>
-    <t>In Arbeit</t>
+    <t>8.Userstory</t>
+  </si>
+  <si>
+    <t>Als Benutzer soll man die Möglichkeit haben zwischen den Sprachen Deutsch und Englisch zu wählen</t>
   </si>
 </sst>
 </file>
@@ -297,14 +300,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -314,6 +317,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -597,7 +601,7 @@
   <dimension ref="C3:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,6 +744,12 @@
       </c>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
       <c r="O11" t="s">
         <v>6</v>
       </c>
@@ -881,48 +891,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353FBFB2-16BE-4644-9382-36A3ABDFA74F}">
-  <dimension ref="C3:J10"/>
+  <dimension ref="C3:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="2"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
@@ -930,59 +940,55 @@
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C7:I7"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -991,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
   <dimension ref="B4:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,7 +1070,7 @@
       <c r="K8" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>43515</v>
       </c>
       <c r="M8" t="s">
@@ -1081,7 +1087,7 @@
       <c r="K9" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>43515</v>
       </c>
       <c r="M9" t="s">
@@ -1098,7 +1104,7 @@
       <c r="K10" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>43515</v>
       </c>
       <c r="M10" t="s">
@@ -1115,7 +1121,7 @@
       <c r="K11" t="s">
         <v>49</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>43517</v>
       </c>
       <c r="M11" t="s">
@@ -1137,21 +1143,21 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
       <c r="K14" t="s">
         <v>50</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="2">
         <v>43515</v>
       </c>
       <c r="M14" t="s">
@@ -1168,7 +1174,7 @@
       <c r="K15" t="s">
         <v>50</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="2">
         <v>43515</v>
       </c>
       <c r="M15" t="s">
@@ -1185,7 +1191,7 @@
       <c r="K16" t="s">
         <v>50</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="2">
         <v>43515</v>
       </c>
       <c r="M16" t="s">
@@ -1202,7 +1208,7 @@
       <c r="K17" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="2">
         <v>43522</v>
       </c>
       <c r="M17" t="s">
@@ -1219,11 +1225,11 @@
       <c r="K18" t="s">
         <v>50</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="2">
         <v>43522</v>
       </c>
       <c r="M18" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="3:18" x14ac:dyDescent="0.3">
@@ -1236,7 +1242,7 @@
       <c r="K19" t="s">
         <v>50</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="2">
         <v>43515</v>
       </c>
       <c r="M19" t="s">
@@ -1256,6 +1262,15 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
+      <c r="K20" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M20" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.3">
       <c r="L21" s="5"/>
@@ -1295,16 +1310,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L22:R22"/>
+    <mergeCell ref="L23:R23"/>
+    <mergeCell ref="L24:R24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="D20:J20"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="L21:R21"/>
-    <mergeCell ref="L22:R22"/>
-    <mergeCell ref="L23:R23"/>
-    <mergeCell ref="L24:R24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="D20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Die View für das Anzeigen aller registrierten Benutzer erstellt und ebenfalls die Methode erstellt um alle Benutzer in schöner Form anzuzeigen
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F85BF5-B319-4AE4-BAD2-0F1AFA467A2E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC82AC5-9306-4476-A5CF-CE8883CB9C44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
   <si>
     <t>Userstories</t>
   </si>
@@ -247,6 +247,30 @@
   </si>
   <si>
     <t>Als Benutzer soll man die Möglichkeit haben zwischen den Sprachen Deutsch und Englisch zu wählen</t>
+  </si>
+  <si>
+    <t>1.Task</t>
+  </si>
+  <si>
+    <t>2.Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.Task </t>
+  </si>
+  <si>
+    <t>Die Navigation.cshtml schreiben und die entsprechenden Links hinzufügen</t>
+  </si>
+  <si>
+    <t>auf der Message-View nach dem Registrieren soll ein Button sein mit dem man zum Login kommt</t>
+  </si>
+  <si>
+    <t>auf dem Hauptlayout soll ein Button erstellt werden mit dem man immer auf die Homeseite kommt</t>
+  </si>
+  <si>
+    <t>View für die Benutzerverwaltung erstellen</t>
+  </si>
+  <si>
+    <t>Die Methode schreiben um alle User zu bekommen</t>
   </si>
 </sst>
 </file>
@@ -300,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -308,16 +332,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -598,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:Q27"/>
+  <dimension ref="C3:Q46"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K25" sqref="K25:P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,77 +636,77 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="O6" s="6" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="O6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
       <c r="O7" t="s">
         <v>3</v>
       </c>
@@ -693,15 +718,15 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
       <c r="O8" t="s">
         <v>2</v>
       </c>
@@ -713,15 +738,15 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
       <c r="O9" t="s">
         <v>4</v>
       </c>
@@ -797,7 +822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O17" t="s">
         <v>12</v>
       </c>
@@ -805,7 +830,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O18" t="s">
         <v>13</v>
       </c>
@@ -813,7 +838,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O19" t="s">
         <v>14</v>
       </c>
@@ -821,7 +846,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O20" t="s">
         <v>15</v>
       </c>
@@ -829,7 +854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O21" t="s">
         <v>16</v>
       </c>
@@ -837,7 +862,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O22" t="s">
         <v>17</v>
       </c>
@@ -845,7 +870,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O23" t="s">
         <v>18</v>
       </c>
@@ -853,36 +878,185 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="15:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:16" x14ac:dyDescent="0.3">
       <c r="O24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O25" t="s">
+    <row r="25" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K25" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+    </row>
+    <row r="26" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K26" t="s">
+        <v>3</v>
+      </c>
+      <c r="L26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K27" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K29" t="s">
+        <v>5</v>
+      </c>
+      <c r="L29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K31" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="11:16" x14ac:dyDescent="0.3">
+      <c r="K32" t="s">
+        <v>8</v>
+      </c>
+      <c r="L32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K33" t="s">
+        <v>9</v>
+      </c>
+      <c r="L33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K36" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K37" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K39" t="s">
+        <v>15</v>
+      </c>
+      <c r="L39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K40" t="s">
+        <v>16</v>
+      </c>
+      <c r="L40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K41" t="s">
+        <v>17</v>
+      </c>
+      <c r="L41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K42" t="s">
+        <v>18</v>
+      </c>
+      <c r="L42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K44" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O26" t="s">
+    <row r="45" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K45" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.3">
-      <c r="O27" t="s">
+    <row r="46" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K46" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
+  <mergeCells count="9">
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="D6:J6"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -893,22 +1067,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353FBFB2-16BE-4644-9382-36A3ABDFA74F}">
   <dimension ref="C3:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
@@ -995,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R24"/>
+  <dimension ref="B4:R29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,34 +1182,34 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
       <c r="K6" t="s">
         <v>48</v>
       </c>
@@ -1050,15 +1224,15 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
@@ -1132,15 +1306,15 @@
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
@@ -1198,7 +1372,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>60</v>
       </c>
@@ -1215,7 +1389,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>62</v>
       </c>
@@ -1232,7 +1406,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>64</v>
       </c>
@@ -1249,77 +1423,142 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" t="s">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="K23" t="s">
         <v>50</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L23" s="6">
         <v>43522</v>
       </c>
-      <c r="M20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
+      <c r="M23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L24" s="6"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="K28" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="L22:R22"/>
-    <mergeCell ref="L23:R23"/>
-    <mergeCell ref="L24:R24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
+  <mergeCells count="8">
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="L21:R21"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sessions kontrolliert und die Unterscheidung beim Login möglich gemacht
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC82AC5-9306-4476-A5CF-CE8883CB9C44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6768D87-83AE-43F9-BCE8-58D5D631F75B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="93">
   <si>
     <t>Userstories</t>
   </si>
@@ -271,6 +271,36 @@
   </si>
   <si>
     <t>Die Methode schreiben um alle User zu bekommen</t>
+  </si>
+  <si>
+    <t>3.Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es soll zwischen den verschiedenen Userrollen unterschieden werden </t>
+  </si>
+  <si>
+    <t xml:space="preserve">in Arbeit </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.Task </t>
+  </si>
+  <si>
+    <t>Neben jeden User in der Liste soll ein Button zum Löschen des Benutzers sein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein Admin soll über ein Suchfeld nach der ID oder dem Nachnamen suchen können </t>
+  </si>
+  <si>
+    <t>6. Task</t>
+  </si>
+  <si>
+    <t>Der User Klasse soll ein Feld hinzugefügt werden ob ein Benutzer gesperrt ist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenn ein Benutzer vom Admin als gesperrt erklärt wurde, soll er sich nicht mehr anmelden können </t>
   </si>
 </sst>
 </file>
@@ -1048,15 +1078,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="D6:J6"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D5:J5"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1169,9 +1199,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R29"/>
+  <dimension ref="B4:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
@@ -1436,6 +1466,9 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
+      <c r="K20" t="s">
+        <v>86</v>
+      </c>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
@@ -1497,6 +1530,9 @@
       <c r="D24" t="s">
         <v>80</v>
       </c>
+      <c r="K24" t="s">
+        <v>86</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -1512,6 +1548,9 @@
       <c r="D25" t="s">
         <v>78</v>
       </c>
+      <c r="K25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
@@ -1531,6 +1570,9 @@
       <c r="K28" t="s">
         <v>50</v>
       </c>
+      <c r="L28" s="2">
+        <v>43516</v>
+      </c>
       <c r="M28" t="s">
         <v>55</v>
       </c>
@@ -1545,20 +1587,105 @@
       <c r="K29" t="s">
         <v>50</v>
       </c>
+      <c r="L29" s="2">
+        <v>43516</v>
+      </c>
       <c r="M29" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>84</v>
+      </c>
+      <c r="K30" t="s">
+        <v>49</v>
+      </c>
+      <c r="L30" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" t="s">
+        <v>88</v>
+      </c>
+      <c r="K31" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+      <c r="K32" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" t="s">
+        <v>91</v>
+      </c>
+      <c r="K33" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>92</v>
+      </c>
+      <c r="K34" t="s">
+        <v>49</v>
+      </c>
+      <c r="L34" s="2">
+        <v>43522</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="L21:R21"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="D20:J20"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Es ist möglich einen Benutzer zu sperren
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6768D87-83AE-43F9-BCE8-58D5D631F75B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B66F22-CE23-43A8-8D9D-9FFDBE9223B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="93">
   <si>
     <t>Userstories</t>
   </si>
@@ -291,16 +291,16 @@
     <t>Neben jeden User in der Liste soll ein Button zum Löschen des Benutzers sein</t>
   </si>
   <si>
-    <t xml:space="preserve">Ein Admin soll über ein Suchfeld nach der ID oder dem Nachnamen suchen können </t>
-  </si>
-  <si>
     <t>6. Task</t>
   </si>
   <si>
     <t>Der User Klasse soll ein Feld hinzugefügt werden ob ein Benutzer gesperrt ist</t>
   </si>
   <si>
-    <t xml:space="preserve">Wenn ein Benutzer vom Admin als gesperrt erklärt wurde, soll er sich nicht mehr anmelden können </t>
+    <t xml:space="preserve">Als Admin soll man einen Benutzer sperren und löschen können </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein Admin soll über ein Suchfeld nach der Vorname oder dem Nachnamen suchen können </t>
   </si>
 </sst>
 </file>
@@ -1078,15 +1078,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:J5"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="D8:J8"/>
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="C3:J3"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1199,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R34"/>
+  <dimension ref="B4:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,10 +1633,10 @@
         <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L32" s="2">
         <v>43522</v>
@@ -1647,10 +1647,10 @@
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
         <v>90</v>
-      </c>
-      <c r="D33" t="s">
-        <v>91</v>
       </c>
       <c r="K33" t="s">
         <v>50</v>
@@ -1667,25 +1667,31 @@
         <v>67</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L34" s="2">
         <v>43522</v>
       </c>
+      <c r="M34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="L35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="L21:R21"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="D20:J20"/>
     <mergeCell ref="C22:I22"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
-    <mergeCell ref="L21:R21"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="D20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Hinzugefügt, dass mit Logout die Session wieder zurückgesetzt wird
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B66F22-CE23-43A8-8D9D-9FFDBE9223B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FB2938-14C1-4BA0-B8AD-646765C13791}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="104">
   <si>
     <t>Userstories</t>
   </si>
@@ -301,6 +301,39 @@
   </si>
   <si>
     <t xml:space="preserve">Ein Admin soll über ein Suchfeld nach der Vorname oder dem Nachnamen suchen können </t>
+  </si>
+  <si>
+    <t>8. Task</t>
+  </si>
+  <si>
+    <t>Seiten auf die nur ein Admin Zutritt hat, soll auch nur der Admin hinkommen</t>
+  </si>
+  <si>
+    <t>Wenn man die Webseite aufruft soll man nur auf die Login kommen</t>
+  </si>
+  <si>
+    <t>9. Task</t>
+  </si>
+  <si>
+    <t>Wenn man bevor man sich angemeldet hat eine andere URL eingibt soll man wieder zur Login kommen</t>
+  </si>
+  <si>
+    <t>10.Task</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll eine Fehlermeldung bekommen wenn die Email schon vergeben ist</t>
+  </si>
+  <si>
+    <t>Als Admin soll man einen Link haben um das Layout der Seite zu ändern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Task </t>
+  </si>
+  <si>
+    <t>Wenn der Benutzer sich ausloggt, soll die Logout aufgerufen werden und die Session null sein</t>
+  </si>
+  <si>
+    <t>Eine View erstellen um das Layout der Seite zu ändern</t>
   </si>
 </sst>
 </file>
@@ -354,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -364,6 +397,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -666,77 +705,77 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="O6" s="7" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="O6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
       <c r="O7" t="s">
         <v>3</v>
       </c>
@@ -748,15 +787,15 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
       <c r="O8" t="s">
         <v>2</v>
       </c>
@@ -768,15 +807,15 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
       <c r="O9" t="s">
         <v>4</v>
       </c>
@@ -914,11 +953,11 @@
       </c>
     </row>
     <row r="25" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
     </row>
     <row r="26" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K26" t="s">
@@ -1098,7 +1137,7 @@
   <dimension ref="C3:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1199,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R35"/>
+  <dimension ref="B4:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,34 +1251,34 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
       <c r="K6" t="s">
         <v>48</v>
       </c>
@@ -1254,15 +1293,15 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
@@ -1336,15 +1375,15 @@
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
@@ -1457,172 +1496,178 @@
       <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
       <c r="K20" t="s">
         <v>86</v>
       </c>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M21" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K22" t="s">
+        <v>50</v>
+      </c>
+      <c r="L22" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M22" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+      <c r="K23" t="s">
+        <v>50</v>
+      </c>
+      <c r="L23" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
         <v>75</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>79</v>
       </c>
-      <c r="K23" t="s">
-        <v>50</v>
-      </c>
-      <c r="L23" s="6">
+      <c r="K26" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="6">
         <v>43522</v>
       </c>
-      <c r="M23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
+      <c r="M26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>80</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K27" t="s">
         <v>86</v>
       </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" t="s">
-        <v>78</v>
-      </c>
-      <c r="K25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>28</v>
-      </c>
+      <c r="L27" s="6"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K28" t="s">
-        <v>50</v>
-      </c>
-      <c r="L28" s="2">
-        <v>43516</v>
-      </c>
-      <c r="M28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" t="s">
-        <v>82</v>
-      </c>
-      <c r="K29" t="s">
-        <v>50</v>
-      </c>
-      <c r="L29" s="2">
-        <v>43516</v>
-      </c>
-      <c r="M29" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
       <c r="C30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" t="s">
-        <v>84</v>
-      </c>
-      <c r="K30" t="s">
-        <v>49</v>
-      </c>
-      <c r="L30" s="2">
-        <v>43522</v>
-      </c>
-      <c r="M30" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="K31" t="s">
         <v>50</v>
       </c>
       <c r="L31" s="2">
-        <v>43522</v>
+        <v>43516</v>
       </c>
       <c r="M31" t="s">
         <v>55</v>
@@ -1630,44 +1675,44 @@
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="K32" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="2">
+        <v>43516</v>
+      </c>
+      <c r="M32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" t="s">
         <v>49</v>
-      </c>
-      <c r="L32" s="2">
-        <v>43522</v>
-      </c>
-      <c r="M32" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" t="s">
-        <v>90</v>
-      </c>
-      <c r="K33" t="s">
-        <v>50</v>
       </c>
       <c r="L33" s="2">
         <v>43522</v>
       </c>
       <c r="M33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K34" t="s">
         <v>50</v>
@@ -1676,18 +1721,139 @@
         <v>43522</v>
       </c>
       <c r="M34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" t="s">
+        <v>92</v>
+      </c>
+      <c r="K35" t="s">
+        <v>49</v>
+      </c>
+      <c r="L35" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="L35" s="2"/>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" t="s">
+        <v>90</v>
+      </c>
+      <c r="K36" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" t="s">
+        <v>91</v>
+      </c>
+      <c r="K37" t="s">
+        <v>50</v>
+      </c>
+      <c r="L37" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="K38" t="s">
+        <v>50</v>
+      </c>
+      <c r="L38" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" t="s">
+        <v>94</v>
+      </c>
+      <c r="K39" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K42" t="s">
+        <v>49</v>
+      </c>
+      <c r="L42" s="2">
+        <v>43522</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" t="s">
+        <v>103</v>
+      </c>
+      <c r="K43" t="s">
+        <v>50</v>
+      </c>
+      <c r="L43" s="2">
+        <v>43522</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="L21:R21"/>
+    <mergeCell ref="L24:R24"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="D20:J20"/>
-    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C25:I25"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>

</xml_diff>

<commit_message>
ein Admin kann nicht mehr gesperrt oder gelöscht werden
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FB2938-14C1-4BA0-B8AD-646765C13791}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110A8DD0-4FB3-4325-9A0C-58FB0D4266B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1241,7 +1241,7 @@
   <dimension ref="B4:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1842,7 +1842,7 @@
         <v>103</v>
       </c>
       <c r="K43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L43" s="2">
         <v>43522</v>

</xml_diff>

<commit_message>
Der Admin kann einen User wieder entsperren
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110A8DD0-4FB3-4325-9A0C-58FB0D4266B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B10084C-D9B9-45CF-AEC2-9B0CDE01A585}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="108">
   <si>
     <t>Userstories</t>
   </si>
@@ -334,6 +334,18 @@
   </si>
   <si>
     <t>Eine View erstellen um das Layout der Seite zu ändern</t>
+  </si>
+  <si>
+    <t>Ein Admin darf nicht gesperrt oder gelöscht werden</t>
+  </si>
+  <si>
+    <t>10. Task</t>
+  </si>
+  <si>
+    <t>11. Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein Admin soll einen User auch entsperren können </t>
   </si>
 </sst>
 </file>
@@ -1117,15 +1129,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:J5"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="D8:J8"/>
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="C3:J3"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1137,7 +1149,7 @@
   <dimension ref="C3:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R43"/>
+  <dimension ref="B4:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1794,10 +1806,10 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="K39" t="s">
         <v>50</v>
@@ -1810,54 +1822,96 @@
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="L40" s="2"/>
+      <c r="C40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" t="s">
+        <v>94</v>
+      </c>
+      <c r="K40" t="s">
+        <v>50</v>
+      </c>
+      <c r="L40" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M40" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" t="s">
+        <v>107</v>
+      </c>
+      <c r="K41" t="s">
+        <v>50</v>
+      </c>
+      <c r="L41" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C42" s="3" t="s">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D44" t="s">
         <v>100</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K44" t="s">
         <v>49</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L44" s="2">
         <v>43522</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C43" s="3" t="s">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>103</v>
       </c>
-      <c r="K43" t="s">
+      <c r="K45" t="s">
         <v>49</v>
       </c>
-      <c r="L43" s="2">
+      <c r="L45" s="2">
         <v>43522</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="L24:R24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="D20:J20"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
+    <mergeCell ref="L24:R24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="D20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Layout und Userdaten ändern erzeugt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B10084C-D9B9-45CF-AEC2-9B0CDE01A585}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE43C983-5122-4415-967C-C2B9B6BB4A9B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
   <si>
     <t>Userstories</t>
   </si>
@@ -346,6 +346,21 @@
   </si>
   <si>
     <t xml:space="preserve">Ein Admin soll einen User auch entsperren können </t>
+  </si>
+  <si>
+    <t>Es soll eine View erstellt werden, wo die Daten geändert werden können</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll alle seine Daten bearebiten können und mit einem Knopf bestätigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Benutzer soll den Hintergrund deer Login ändern können </t>
+  </si>
+  <si>
+    <t>Der Benutzer soll nur seine und keine anderen Daten bearbeiten können</t>
+  </si>
+  <si>
+    <t>05.03.2019.</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1164,7 @@
   <dimension ref="C3:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R47"/>
+  <dimension ref="B4:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,7 +1591,7 @@
         <v>43522</v>
       </c>
       <c r="M23" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
@@ -1874,10 +1889,10 @@
         <v>100</v>
       </c>
       <c r="K44" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L44" s="2">
-        <v>43522</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
@@ -1888,18 +1903,88 @@
         <v>103</v>
       </c>
       <c r="K45" t="s">
-        <v>49</v>
-      </c>
-      <c r="L45" s="2">
+        <v>50</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>110</v>
+      </c>
+      <c r="K46" t="s">
+        <v>50</v>
+      </c>
+      <c r="L46" s="2">
+        <v>43529</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C49" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" t="s">
+        <v>108</v>
+      </c>
+      <c r="K49" t="s">
+        <v>50</v>
+      </c>
+      <c r="L49" s="2">
         <v>43522</v>
       </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>39</v>
+      <c r="M49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C50" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" t="s">
+        <v>109</v>
+      </c>
+      <c r="K50" t="s">
+        <v>50</v>
+      </c>
+      <c r="L50" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C51" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" t="s">
+        <v>111</v>
+      </c>
+      <c r="K51" t="s">
+        <v>50</v>
+      </c>
+      <c r="L51" s="2">
+        <v>43529</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Benutzer kann den Hintergrund der Loginseite ändern
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE43C983-5122-4415-967C-C2B9B6BB4A9B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF6F0E9-5E37-48B2-B5AD-118F48608D02}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="112">
   <si>
     <t>Userstories</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Als Benutzer soll man sich mit einfachen Buttons durch die komplette Seite klicken können</t>
   </si>
   <si>
-    <t>in Arbeit</t>
-  </si>
-  <si>
     <t>responsive Design bei allen Layouts</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t xml:space="preserve">Es soll zwischen den verschiedenen Userrollen unterschieden werden </t>
   </si>
   <si>
-    <t xml:space="preserve">in Arbeit </t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -361,6 +355,9 @@
   </si>
   <si>
     <t>05.03.2019.</t>
+  </si>
+  <si>
+    <t>Der Benutezr soll nur sein Layout ändern können und die ID nicht eingeben müssen</t>
   </si>
 </sst>
 </file>
@@ -866,10 +863,10 @@
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
         <v>73</v>
-      </c>
-      <c r="D11" t="s">
-        <v>74</v>
       </c>
       <c r="O11" t="s">
         <v>6</v>
@@ -1144,15 +1141,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:J5"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="D8:J8"/>
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="C3:J3"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1255,7 +1252,7 @@
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1265,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R54"/>
+  <dimension ref="B4:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1386,7 +1383,7 @@
         <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K11" t="s">
         <v>49</v>
@@ -1395,7 +1392,7 @@
         <v>43517</v>
       </c>
       <c r="M11" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
@@ -1533,16 +1530,16 @@
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1562,10 +1559,10 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K22" t="s">
         <v>50</v>
@@ -1579,10 +1576,10 @@
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K23" t="s">
         <v>50</v>
@@ -1626,10 +1623,10 @@
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K26" t="s">
         <v>50</v>
@@ -1648,16 +1645,18 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K27" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="L27" s="6"/>
-      <c r="M27" s="3"/>
+      <c r="M27" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -1666,13 +1665,13 @@
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" t="s">
         <v>77</v>
       </c>
-      <c r="D28" t="s">
-        <v>78</v>
-      </c>
       <c r="K28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
@@ -1688,7 +1687,7 @@
         <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K31" t="s">
         <v>50</v>
@@ -1705,7 +1704,7 @@
         <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K32" t="s">
         <v>50</v>
@@ -1719,10 +1718,10 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
         <v>83</v>
-      </c>
-      <c r="D33" t="s">
-        <v>84</v>
       </c>
       <c r="K33" t="s">
         <v>49</v>
@@ -1736,10 +1735,10 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K34" t="s">
         <v>50</v>
@@ -1756,7 +1755,7 @@
         <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K35" t="s">
         <v>49</v>
@@ -1765,15 +1764,15 @@
         <v>43522</v>
       </c>
       <c r="M35" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K36" t="s">
         <v>50</v>
@@ -1790,7 +1789,7 @@
         <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K37" t="s">
         <v>50</v>
@@ -1804,10 +1803,10 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K38" t="s">
         <v>50</v>
@@ -1821,10 +1820,10 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K39" t="s">
         <v>50</v>
@@ -1838,10 +1837,10 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K40" t="s">
         <v>50</v>
@@ -1855,10 +1854,10 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K41" t="s">
         <v>50</v>
@@ -1886,7 +1885,7 @@
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K44" t="s">
         <v>50</v>
@@ -1897,63 +1896,58 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" t="s">
         <v>101</v>
       </c>
-      <c r="D45" t="s">
-        <v>103</v>
-      </c>
       <c r="K45" t="s">
         <v>50</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" t="s">
+        <v>111</v>
+      </c>
+      <c r="K46" t="s">
+        <v>50</v>
+      </c>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C47" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D46" t="s">
-        <v>110</v>
-      </c>
-      <c r="K46" t="s">
-        <v>50</v>
-      </c>
-      <c r="L46" s="2">
+      <c r="D47" t="s">
+        <v>108</v>
+      </c>
+      <c r="K47" t="s">
+        <v>50</v>
+      </c>
+      <c r="L47" s="2">
         <v>43529</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C49" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" t="s">
-        <v>108</v>
-      </c>
-      <c r="K49" t="s">
-        <v>50</v>
-      </c>
-      <c r="L49" s="2">
-        <v>43522</v>
-      </c>
-      <c r="M49" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C50" s="3" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K50" t="s">
         <v>50</v>
@@ -1967,36 +1961,53 @@
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" t="s">
+        <v>107</v>
+      </c>
+      <c r="K51" t="s">
+        <v>50</v>
+      </c>
+      <c r="L51" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D51" t="s">
-        <v>111</v>
-      </c>
-      <c r="K51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L51" s="2">
+      <c r="D52" t="s">
+        <v>109</v>
+      </c>
+      <c r="K52" t="s">
+        <v>50</v>
+      </c>
+      <c r="L52" s="2">
         <v>43529</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="L24:R24"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="D20:J20"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
-    <mergeCell ref="L24:R24"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="D20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sidenav wurde hinzugefügt und der richtige Name sowie die richtige Email werden in der Sidenav angezeigt und der Admin hat zusätzliche Links
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220FD74E-7E3E-4023-B564-85A81178D46A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920960F1-C894-4F32-8883-8B571F5FFFBC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="131">
   <si>
     <t>Userstories</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Als Benutzer soll man einen Link haben um das Layout der Seite zu ändern</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll die Möglichkeit haben ein Profilbild einzustellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es soll eine Sidenav eingefügt werden </t>
   </si>
 </sst>
 </file>
@@ -480,6 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,7 +499,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -786,77 +792,77 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="O6" s="6" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="O6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
       <c r="O7" t="s">
         <v>3</v>
       </c>
@@ -868,15 +874,15 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
       <c r="O8" t="s">
         <v>2</v>
       </c>
@@ -888,15 +894,15 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
       <c r="O9" t="s">
         <v>4</v>
       </c>
@@ -1034,11 +1040,11 @@
       </c>
     </row>
     <row r="25" spans="11:16" x14ac:dyDescent="0.3">
-      <c r="K25" s="6" t="s">
+      <c r="K25" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
     </row>
     <row r="26" spans="11:16" x14ac:dyDescent="0.3">
       <c r="K26" t="s">
@@ -1198,15 +1204,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="D6:J6"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1283,10 +1289,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R73"/>
+  <dimension ref="B4:R75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1299,34 +1305,34 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
       <c r="K6" t="s">
         <v>48</v>
       </c>
@@ -1341,15 +1347,15 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
@@ -1420,21 +1426,21 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M12" s="10"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
@@ -1542,15 +1548,15 @@
       <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
       <c r="K20" t="s">
         <v>85</v>
       </c>
@@ -1614,99 +1620,99 @@
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
+        <v>129</v>
+      </c>
+      <c r="K24" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="2">
+        <v>43543</v>
+      </c>
+      <c r="M24" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" t="s">
-        <v>79</v>
-      </c>
-      <c r="K26" t="s">
-        <v>50</v>
-      </c>
-      <c r="L26" s="2">
-        <v>43522</v>
-      </c>
-      <c r="M26" t="s">
-        <v>55</v>
-      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K27" t="s">
-        <v>85</v>
-      </c>
-      <c r="L27" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="L27" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M27" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K28" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="K29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" t="s">
-        <v>81</v>
-      </c>
-      <c r="K31" t="s">
-        <v>50</v>
-      </c>
-      <c r="L31" s="2">
-        <v>43516</v>
-      </c>
-      <c r="M31" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K32" t="s">
         <v>50</v>
@@ -1720,16 +1726,16 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L33" s="2">
-        <v>43522</v>
+        <v>43516</v>
       </c>
       <c r="M33" t="s">
         <v>55</v>
@@ -1737,13 +1743,13 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L34" s="2">
         <v>43522</v>
@@ -1754,13 +1760,13 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L35" s="2">
         <v>43522</v>
@@ -1771,13 +1777,13 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L36" s="2">
         <v>43522</v>
@@ -1788,10 +1794,10 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K37" t="s">
         <v>50</v>
@@ -1805,10 +1811,10 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K38" t="s">
         <v>50</v>
@@ -1822,10 +1828,10 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K39" t="s">
         <v>50</v>
@@ -1839,10 +1845,10 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="K40" t="s">
         <v>50</v>
@@ -1856,10 +1862,10 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="K41" t="s">
         <v>50</v>
@@ -1872,56 +1878,56 @@
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="L42" s="2"/>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" t="s">
+        <v>105</v>
+      </c>
+      <c r="K42" t="s">
+        <v>50</v>
+      </c>
+      <c r="L42" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M42" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" t="s">
+        <v>130</v>
+      </c>
+      <c r="K43" t="s">
+        <v>50</v>
+      </c>
+      <c r="L43" s="2">
+        <v>43549</v>
+      </c>
+      <c r="M43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>6</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" t="s">
-        <v>128</v>
-      </c>
-      <c r="K44" t="s">
-        <v>50</v>
-      </c>
-      <c r="L44" s="2">
-        <v>43536</v>
-      </c>
-      <c r="M44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" t="s">
-        <v>101</v>
-      </c>
-      <c r="K45" t="s">
-        <v>50</v>
-      </c>
-      <c r="L45" s="2">
-        <v>43536</v>
-      </c>
-      <c r="M45" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="K46" t="s">
         <v>50</v>
@@ -1933,174 +1939,177 @@
         <v>55</v>
       </c>
     </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" t="s">
+        <v>101</v>
+      </c>
+      <c r="K47" t="s">
+        <v>50</v>
+      </c>
+      <c r="L47" s="2">
+        <v>43536</v>
+      </c>
+      <c r="M47" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+      <c r="C48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" t="s">
+        <v>108</v>
+      </c>
+      <c r="K48" t="s">
+        <v>50</v>
+      </c>
+      <c r="L48" s="2">
+        <v>43536</v>
+      </c>
+      <c r="M48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>7</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" t="s">
-        <v>106</v>
-      </c>
-      <c r="K49" t="s">
-        <v>50</v>
-      </c>
-      <c r="L49" s="2">
-        <v>43522</v>
-      </c>
-      <c r="M49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" t="s">
-        <v>107</v>
-      </c>
-      <c r="K50" t="s">
-        <v>50</v>
-      </c>
-      <c r="L50" s="2">
-        <v>43522</v>
-      </c>
-      <c r="M50" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" t="s">
+        <v>106</v>
+      </c>
+      <c r="K51" t="s">
+        <v>50</v>
+      </c>
+      <c r="L51" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" t="s">
+        <v>107</v>
+      </c>
+      <c r="K52" t="s">
+        <v>50</v>
+      </c>
+      <c r="L52" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
         <v>52</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D53" t="s">
         <v>109</v>
       </c>
-      <c r="K51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L51" s="2">
+      <c r="K53" t="s">
+        <v>50</v>
+      </c>
+      <c r="L53" s="2">
         <v>43536</v>
       </c>
-      <c r="M51" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
+      <c r="M53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
         <v>8</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C55" s="9" t="s">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C57" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" t="s">
-        <v>110</v>
-      </c>
-      <c r="K56" t="s">
-        <v>49</v>
-      </c>
-      <c r="L56" s="2">
-        <v>43529</v>
-      </c>
-      <c r="M56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" t="s">
-        <v>111</v>
-      </c>
-      <c r="K57" t="s">
-        <v>49</v>
-      </c>
-      <c r="L57" s="2">
-        <v>43536</v>
-      </c>
-      <c r="M57" t="s">
-        <v>55</v>
-      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D58" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K58" t="s">
         <v>49</v>
       </c>
       <c r="L58" s="2">
-        <v>43543</v>
+        <v>43529</v>
       </c>
       <c r="M58" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K59" t="s">
         <v>49</v>
       </c>
       <c r="L59" s="2">
-        <v>43543</v>
+        <v>43536</v>
       </c>
       <c r="M59" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L60" s="2">
-        <v>43550</v>
+        <v>43543</v>
+      </c>
+      <c r="M60" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K61" t="s">
         <v>49</v>
       </c>
       <c r="L61" s="2">
-        <v>43529</v>
+        <v>43543</v>
       </c>
       <c r="M61" t="s">
         <v>71</v>
@@ -2108,127 +2117,158 @@
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K62" t="s">
         <v>50</v>
       </c>
       <c r="L62" s="2">
-        <v>43543</v>
+        <v>43550</v>
       </c>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D63" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L63" s="2">
-        <v>43543</v>
+        <v>43550</v>
+      </c>
+      <c r="M63" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C64" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
+      <c r="C64" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" t="s">
+        <v>116</v>
+      </c>
+      <c r="K64" t="s">
+        <v>50</v>
+      </c>
+      <c r="L64" s="2">
+        <v>43550</v>
+      </c>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K65" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L65" s="2">
-        <v>43557</v>
+        <v>43550</v>
       </c>
     </row>
     <row r="66" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>103</v>
-      </c>
-      <c r="D66" t="s">
-        <v>122</v>
-      </c>
-      <c r="K66" t="s">
-        <v>50</v>
-      </c>
-      <c r="L66" s="2">
-        <v>43557</v>
-      </c>
+      <c r="C66" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
     </row>
     <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D67" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K67" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L67" s="2">
         <v>43557</v>
       </c>
     </row>
-    <row r="71" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C71" s="9" t="s">
+    <row r="68" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" t="s">
+        <v>122</v>
+      </c>
+      <c r="K68" t="s">
+        <v>50</v>
+      </c>
+      <c r="L68" s="2">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="69" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>104</v>
+      </c>
+      <c r="D69" t="s">
+        <v>125</v>
+      </c>
+      <c r="K69" t="s">
+        <v>50</v>
+      </c>
+      <c r="L69" s="2">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="73" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C73" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-    </row>
-    <row r="72" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C72" t="s">
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+    </row>
+    <row r="74" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
         <v>126</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D74" t="s">
         <v>119</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K74" t="s">
         <v>49</v>
       </c>
-      <c r="L72" s="2">
+      <c r="L74" s="2">
         <v>43557</v>
       </c>
     </row>
-    <row r="73" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C73" t="s">
+    <row r="75" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
         <v>127</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D75" t="s">
         <v>124</v>
       </c>
-      <c r="K73" t="s">
+      <c r="K75" t="s">
         <v>49</v>
       </c>
-      <c r="L73" s="2">
+      <c r="L75" s="2">
         <v>43564</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C26:I26"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
-    <mergeCell ref="L24:R24"/>
+    <mergeCell ref="L25:R25"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="D20:J20"/>
   </mergeCells>

</xml_diff>

<commit_message>
Vorausgefüllte Werte beim Datenändern
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920960F1-C894-4F32-8883-8B571F5FFFBC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D926ECA3-9259-48A1-A771-8B7D760837BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="132">
   <si>
     <t>Userstories</t>
   </si>
@@ -255,12 +255,6 @@
     <t>2.Task</t>
   </si>
   <si>
-    <t xml:space="preserve">3.Task </t>
-  </si>
-  <si>
-    <t>Die Navigation.cshtml schreiben und die entsprechenden Links hinzufügen</t>
-  </si>
-  <si>
     <t>auf der Message-View nach dem Registrieren soll ein Button sein mit dem man zum Login kommt</t>
   </si>
   <si>
@@ -369,12 +363,6 @@
     <t>der Benutzer soll andere Posts sehen, liken und kommentieren können (Feed)</t>
   </si>
   <si>
-    <t>Es soll dem Benutzer möglich sein, andere Benutzer im Beitrag zu markieren</t>
-  </si>
-  <si>
-    <t>Freunde und Benachrichtigungen sollen vom Benutzer über Tabs ersichtlich sein</t>
-  </si>
-  <si>
     <t>Feed und Hauptseite</t>
   </si>
   <si>
@@ -415,6 +403,21 @@
   </si>
   <si>
     <t xml:space="preserve">Es soll eine Sidenav eingefügt werden </t>
+  </si>
+  <si>
+    <t>26:02:2019</t>
+  </si>
+  <si>
+    <t>Die entsprechenden Links auf der Sidenav setzen und nur der Admin soll Zusatzlinks haben</t>
+  </si>
+  <si>
+    <t>4.Task</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll seine Daten beim Daten ändern nicht selbst eingeben müssen</t>
+  </si>
+  <si>
+    <t>Freunde sollen vom Benutzer über Tabs ersichtlich sein</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1204,15 +1207,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="D6:J6"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D5:J5"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1289,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
-  <dimension ref="B4:R75"/>
+  <dimension ref="B4:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,14 +1308,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D5" s="8"/>
@@ -1558,16 +1561,16 @@
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1587,10 +1590,10 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K22" t="s">
         <v>50</v>
@@ -1604,10 +1607,10 @@
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K23" t="s">
         <v>50</v>
@@ -1621,10 +1624,10 @@
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K24" t="s">
         <v>50</v>
@@ -1633,7 +1636,7 @@
         <v>43543</v>
       </c>
       <c r="M24" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
@@ -1664,7 +1667,7 @@
         <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K27" t="s">
         <v>50</v>
@@ -1681,22 +1684,16 @@
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K28" t="s">
-        <v>85</v>
-      </c>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" t="s">
-        <v>78</v>
-      </c>
-      <c r="K29" t="s">
-        <v>85</v>
+        <v>50</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M28" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
@@ -1712,7 +1709,7 @@
         <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K32" t="s">
         <v>50</v>
@@ -1729,7 +1726,7 @@
         <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K33" t="s">
         <v>50</v>
@@ -1743,10 +1740,10 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K34" t="s">
         <v>49</v>
@@ -1760,10 +1757,10 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K35" t="s">
         <v>50</v>
@@ -1780,7 +1777,7 @@
         <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K36" t="s">
         <v>49</v>
@@ -1794,10 +1791,10 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K37" t="s">
         <v>50</v>
@@ -1814,7 +1811,7 @@
         <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K38" t="s">
         <v>50</v>
@@ -1828,10 +1825,10 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K39" t="s">
         <v>50</v>
@@ -1845,10 +1842,10 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K40" t="s">
         <v>50</v>
@@ -1862,10 +1859,10 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K41" t="s">
         <v>50</v>
@@ -1879,10 +1876,10 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K42" t="s">
         <v>50</v>
@@ -1896,10 +1893,10 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" t="s">
         <v>126</v>
-      </c>
-      <c r="D43" t="s">
-        <v>130</v>
       </c>
       <c r="K43" t="s">
         <v>50</v>
@@ -1912,39 +1909,39 @@
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="L44" s="2"/>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
+        <v>128</v>
+      </c>
+      <c r="K44" t="s">
+        <v>50</v>
+      </c>
+      <c r="L44" s="2">
+        <v>43549</v>
+      </c>
+      <c r="M44" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>6</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" t="s">
-        <v>128</v>
-      </c>
-      <c r="K46" t="s">
-        <v>50</v>
-      </c>
-      <c r="L46" s="2">
-        <v>43536</v>
-      </c>
-      <c r="M46" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="K47" t="s">
         <v>50</v>
@@ -1958,10 +1955,10 @@
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="K48" t="s">
         <v>50</v>
@@ -1973,37 +1970,37 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" t="s">
+        <v>106</v>
+      </c>
+      <c r="K49" t="s">
+        <v>50</v>
+      </c>
+      <c r="L49" s="2">
+        <v>43536</v>
+      </c>
+      <c r="M49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
         <v>7</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
-        <v>43</v>
-      </c>
-      <c r="D51" t="s">
-        <v>106</v>
-      </c>
-      <c r="K51" t="s">
-        <v>50</v>
-      </c>
-      <c r="L51" s="2">
-        <v>43522</v>
-      </c>
-      <c r="M51" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K52" t="s">
         <v>50</v>
@@ -2017,130 +2014,133 @@
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" t="s">
+        <v>105</v>
+      </c>
+      <c r="K53" t="s">
+        <v>50</v>
+      </c>
+      <c r="L53" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
         <v>52</v>
       </c>
-      <c r="D53" t="s">
-        <v>109</v>
-      </c>
-      <c r="K53" t="s">
-        <v>50</v>
-      </c>
-      <c r="L53" s="2">
+      <c r="D54" t="s">
+        <v>107</v>
+      </c>
+      <c r="K54" t="s">
+        <v>50</v>
+      </c>
+      <c r="L54" s="2">
         <v>43536</v>
       </c>
-      <c r="M53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
+      <c r="M54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" t="s">
+        <v>130</v>
+      </c>
+      <c r="K55" t="s">
+        <v>50</v>
+      </c>
+      <c r="L55" s="2">
+        <v>43550</v>
+      </c>
+      <c r="M55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
         <v>8</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C57" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
-        <v>43</v>
-      </c>
-      <c r="D58" t="s">
-        <v>110</v>
-      </c>
-      <c r="K58" t="s">
-        <v>49</v>
-      </c>
-      <c r="L58" s="2">
-        <v>43529</v>
-      </c>
-      <c r="M58" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
-        <v>46</v>
-      </c>
-      <c r="D59" t="s">
-        <v>111</v>
-      </c>
-      <c r="K59" t="s">
-        <v>49</v>
-      </c>
-      <c r="L59" s="2">
-        <v>43536</v>
-      </c>
-      <c r="M59" t="s">
-        <v>55</v>
-      </c>
+      <c r="C59" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D60" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="K60" t="s">
         <v>49</v>
       </c>
       <c r="L60" s="2">
-        <v>43543</v>
+        <v>43529</v>
       </c>
       <c r="M60" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D61" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K61" t="s">
         <v>49</v>
       </c>
       <c r="L61" s="2">
-        <v>43543</v>
+        <v>43536</v>
       </c>
       <c r="M61" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D62" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L62" s="2">
-        <v>43550</v>
+        <v>43543</v>
+      </c>
+      <c r="M62" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D63" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K63" t="s">
         <v>49</v>
       </c>
       <c r="L63" s="2">
-        <v>43550</v>
+        <v>43543</v>
       </c>
       <c r="M63" t="s">
         <v>71</v>
@@ -2148,10 +2148,10 @@
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K64" t="s">
         <v>50</v>
@@ -2161,116 +2161,133 @@
       </c>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
-        <v>92</v>
-      </c>
-      <c r="D65" t="s">
-        <v>120</v>
-      </c>
-      <c r="K65" t="s">
-        <v>50</v>
-      </c>
-      <c r="L65" s="2">
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>67</v>
+      </c>
+      <c r="D66" t="s">
+        <v>131</v>
+      </c>
+      <c r="K66" t="s">
+        <v>50</v>
+      </c>
+      <c r="L66" s="2">
         <v>43550</v>
       </c>
-    </row>
-    <row r="66" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C66" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
     </row>
     <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D67" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K67" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L67" s="2">
-        <v>43557</v>
+        <v>43550</v>
       </c>
     </row>
     <row r="68" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C68" t="s">
-        <v>103</v>
-      </c>
-      <c r="D68" t="s">
-        <v>122</v>
-      </c>
-      <c r="K68" t="s">
-        <v>50</v>
-      </c>
-      <c r="L68" s="2">
-        <v>43557</v>
-      </c>
+      <c r="C68" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
     </row>
     <row r="69" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D69" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="K69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L69" s="2">
         <v>43557</v>
       </c>
     </row>
-    <row r="73" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C73" s="10" t="s">
+    <row r="70" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>101</v>
+      </c>
+      <c r="D70" t="s">
         <v>118</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-    </row>
-    <row r="74" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C74" t="s">
-        <v>126</v>
-      </c>
-      <c r="D74" t="s">
-        <v>119</v>
-      </c>
-      <c r="K74" t="s">
+      <c r="K70" t="s">
+        <v>50</v>
+      </c>
+      <c r="L70" s="2">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="71" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>102</v>
+      </c>
+      <c r="D71" t="s">
+        <v>121</v>
+      </c>
+      <c r="K71" t="s">
+        <v>50</v>
+      </c>
+      <c r="L71" s="2">
+        <v>43557</v>
+      </c>
+    </row>
+    <row r="75" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C75" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+    </row>
+    <row r="76" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>122</v>
+      </c>
+      <c r="D76" t="s">
+        <v>115</v>
+      </c>
+      <c r="K76" t="s">
         <v>49</v>
       </c>
-      <c r="L74" s="2">
+      <c r="L76" s="2">
         <v>43557</v>
       </c>
     </row>
-    <row r="75" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C75" t="s">
-        <v>127</v>
-      </c>
-      <c r="D75" t="s">
-        <v>124</v>
-      </c>
-      <c r="K75" t="s">
+    <row r="77" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>123</v>
+      </c>
+      <c r="D77" t="s">
+        <v>120</v>
+      </c>
+      <c r="K77" t="s">
         <v>49</v>
       </c>
-      <c r="L75" s="2">
+      <c r="L77" s="2">
         <v>43564</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C7:I7"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="L25:R25"/>
     <mergeCell ref="C13:I13"/>
     <mergeCell ref="D20:J20"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploading/Änderung des Profilbildes hinzugefügt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABF3CA1-9BFC-4D58-A5F2-5FAE9F6E6B97}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE1C6C5-658C-4B98-8CBF-AA5C79281D38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="106">
   <si>
     <t>Userstories</t>
   </si>
@@ -180,175 +180,166 @@
     <t>7. Task</t>
   </si>
   <si>
-    <t>Der Benutzer soll die im Task 6 erzeugten Fehlermeldung in schöner Form angezeigt bekommen</t>
-  </si>
-  <si>
     <t>Als Benutzer soll man sich mit einfachen Buttons durch die komplette Webseite klicken können</t>
   </si>
   <si>
     <t>Als Benutzer soll man sich mit einfachen Buttons durch die komplette Seite klicken können</t>
   </si>
   <si>
+    <t>responsive Design bei allen Layouts</t>
+  </si>
+  <si>
+    <t>1.Task</t>
+  </si>
+  <si>
+    <t>2.Task</t>
+  </si>
+  <si>
+    <t>auf der Message-View nach dem Registrieren soll ein Button sein mit dem man zum Login kommt</t>
+  </si>
+  <si>
+    <t>auf dem Hauptlayout soll ein Button erstellt werden mit dem man immer auf die Homeseite kommt</t>
+  </si>
+  <si>
+    <t>View für die Benutzerverwaltung erstellen</t>
+  </si>
+  <si>
+    <t>Die Methode schreiben um alle User zu bekommen</t>
+  </si>
+  <si>
+    <t>3.Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es soll zwischen den verschiedenen Userrollen unterschieden werden </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.Task </t>
+  </si>
+  <si>
+    <t>Neben jeden User in der Liste soll ein Button zum Löschen des Benutzers sein</t>
+  </si>
+  <si>
+    <t>6. Task</t>
+  </si>
+  <si>
+    <t>Der User Klasse soll ein Feld hinzugefügt werden ob ein Benutzer gesperrt ist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als Admin soll man einen Benutzer sperren und löschen können </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein Admin soll über ein Suchfeld nach der Vorname oder dem Nachnamen suchen können </t>
+  </si>
+  <si>
+    <t>8. Task</t>
+  </si>
+  <si>
+    <t>Seiten auf die nur ein Admin Zutritt hat, soll auch nur der Admin hinkommen</t>
+  </si>
+  <si>
+    <t>Wenn man die Webseite aufruft soll man nur auf die Login kommen</t>
+  </si>
+  <si>
+    <t>9. Task</t>
+  </si>
+  <si>
+    <t>Wenn man bevor man sich angemeldet hat eine andere URL eingibt soll man wieder zur Login kommen</t>
+  </si>
+  <si>
+    <t>10.Task</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll eine Fehlermeldung bekommen wenn die Email schon vergeben ist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Task </t>
+  </si>
+  <si>
+    <t>Wenn der Benutzer sich ausloggt, soll die Logout aufgerufen werden und die Session null sein</t>
+  </si>
+  <si>
+    <t>Eine View erstellen um das Layout der Seite zu ändern</t>
+  </si>
+  <si>
+    <t>Ein Admin darf nicht gesperrt oder gelöscht werden</t>
+  </si>
+  <si>
+    <t>10. Task</t>
+  </si>
+  <si>
+    <t>11. Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein Admin soll einen User auch entsperren können </t>
+  </si>
+  <si>
+    <t>Es soll eine View erstellt werden, wo die Daten geändert werden können</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll alle seine Daten bearebiten können und mit einem Knopf bestätigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Benutzer soll den Hintergrund deer Login ändern können </t>
+  </si>
+  <si>
+    <t>Der Benutzer soll nur seine und keine anderen Daten bearbeiten können</t>
+  </si>
+  <si>
+    <t>eine View (index) für die Feedseite erzeugen</t>
+  </si>
+  <si>
+    <t>ein Layout für einen Feed erzeugen</t>
+  </si>
+  <si>
+    <t>der Benutzer soll eine Fehlermeldung bekommen, wenn der Post zu lang, oder nicht erfolgreich hochgeladen wurde</t>
+  </si>
+  <si>
+    <t>eine Methode zum Beitrag verfassen schreiben</t>
+  </si>
+  <si>
+    <t>der Benutzer soll andere Posts sehen, liken und kommentieren können (Feed)</t>
+  </si>
+  <si>
+    <t>Feed und Hauptseite</t>
+  </si>
+  <si>
+    <t>Man soll Personen über die Suchleiste finden können und dessen Profil ansehen können</t>
+  </si>
+  <si>
+    <t>12. Task</t>
+  </si>
+  <si>
+    <t>13. Task</t>
+  </si>
+  <si>
+    <t>Als Benutzer soll man einen Link haben um das Layout der Seite zu ändern</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll die Möglichkeit haben ein Profilbild einzustellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es soll eine Sidenav eingefügt werden </t>
+  </si>
+  <si>
+    <t>Die entsprechenden Links auf der Sidenav setzen und nur der Admin soll Zusatzlinks haben</t>
+  </si>
+  <si>
+    <t>4.Task</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll seine Daten beim Daten ändern nicht selbst eingeben müssen</t>
+  </si>
+  <si>
+    <t>Freunde sollen vom Benutzer über Tabs ersichtlich sein</t>
+  </si>
+  <si>
+    <t>der Benutzer soll seinen Post nicht hochladen können, wenn der Post zu lang ist</t>
+  </si>
+  <si>
+    <t>Als Benutzer soll man die Möglichkeit haben das Layout der Seite zu ändern</t>
+  </si>
+  <si>
     <t>in Arbeit</t>
-  </si>
-  <si>
-    <t>responsive Design bei allen Layouts</t>
-  </si>
-  <si>
-    <t>1.Task</t>
-  </si>
-  <si>
-    <t>2.Task</t>
-  </si>
-  <si>
-    <t>auf der Message-View nach dem Registrieren soll ein Button sein mit dem man zum Login kommt</t>
-  </si>
-  <si>
-    <t>auf dem Hauptlayout soll ein Button erstellt werden mit dem man immer auf die Homeseite kommt</t>
-  </si>
-  <si>
-    <t>View für die Benutzerverwaltung erstellen</t>
-  </si>
-  <si>
-    <t>Die Methode schreiben um alle User zu bekommen</t>
-  </si>
-  <si>
-    <t>3.Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es soll zwischen den verschiedenen Userrollen unterschieden werden </t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.Task </t>
-  </si>
-  <si>
-    <t>Neben jeden User in der Liste soll ein Button zum Löschen des Benutzers sein</t>
-  </si>
-  <si>
-    <t>6. Task</t>
-  </si>
-  <si>
-    <t>Der User Klasse soll ein Feld hinzugefügt werden ob ein Benutzer gesperrt ist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Als Admin soll man einen Benutzer sperren und löschen können </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ein Admin soll über ein Suchfeld nach der Vorname oder dem Nachnamen suchen können </t>
-  </si>
-  <si>
-    <t>8. Task</t>
-  </si>
-  <si>
-    <t>Seiten auf die nur ein Admin Zutritt hat, soll auch nur der Admin hinkommen</t>
-  </si>
-  <si>
-    <t>Wenn man die Webseite aufruft soll man nur auf die Login kommen</t>
-  </si>
-  <si>
-    <t>9. Task</t>
-  </si>
-  <si>
-    <t>Wenn man bevor man sich angemeldet hat eine andere URL eingibt soll man wieder zur Login kommen</t>
-  </si>
-  <si>
-    <t>10.Task</t>
-  </si>
-  <si>
-    <t>Der Benutzer soll eine Fehlermeldung bekommen wenn die Email schon vergeben ist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Task </t>
-  </si>
-  <si>
-    <t>Wenn der Benutzer sich ausloggt, soll die Logout aufgerufen werden und die Session null sein</t>
-  </si>
-  <si>
-    <t>Eine View erstellen um das Layout der Seite zu ändern</t>
-  </si>
-  <si>
-    <t>Ein Admin darf nicht gesperrt oder gelöscht werden</t>
-  </si>
-  <si>
-    <t>10. Task</t>
-  </si>
-  <si>
-    <t>11. Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ein Admin soll einen User auch entsperren können </t>
-  </si>
-  <si>
-    <t>Es soll eine View erstellt werden, wo die Daten geändert werden können</t>
-  </si>
-  <si>
-    <t>Der Benutzer soll alle seine Daten bearebiten können und mit einem Knopf bestätigen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Benutzer soll den Hintergrund deer Login ändern können </t>
-  </si>
-  <si>
-    <t>Der Benutzer soll nur seine und keine anderen Daten bearbeiten können</t>
-  </si>
-  <si>
-    <t>eine View (index) für die Feedseite erzeugen</t>
-  </si>
-  <si>
-    <t>ein Layout für einen Feed erzeugen</t>
-  </si>
-  <si>
-    <t>der Benutzer soll eine Fehlermeldung bekommen, wenn der Post zu lang, oder nicht erfolgreich hochgeladen wurde</t>
-  </si>
-  <si>
-    <t>eine Methode zum Beitrag verfassen schreiben</t>
-  </si>
-  <si>
-    <t>der Benutzer soll andere Posts sehen, liken und kommentieren können (Feed)</t>
-  </si>
-  <si>
-    <t>Feed und Hauptseite</t>
-  </si>
-  <si>
-    <t>Man soll Personen über die Suchleiste finden können und dessen Profil ansehen können</t>
-  </si>
-  <si>
-    <t>12. Task</t>
-  </si>
-  <si>
-    <t>13. Task</t>
-  </si>
-  <si>
-    <t>Als Benutzer soll man einen Link haben um das Layout der Seite zu ändern</t>
-  </si>
-  <si>
-    <t>Der Benutzer soll die Möglichkeit haben ein Profilbild einzustellen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es soll eine Sidenav eingefügt werden </t>
-  </si>
-  <si>
-    <t>26:02:2019</t>
-  </si>
-  <si>
-    <t>Die entsprechenden Links auf der Sidenav setzen und nur der Admin soll Zusatzlinks haben</t>
-  </si>
-  <si>
-    <t>4.Task</t>
-  </si>
-  <si>
-    <t>Der Benutzer soll seine Daten beim Daten ändern nicht selbst eingeben müssen</t>
-  </si>
-  <si>
-    <t>Freunde sollen vom Benutzer über Tabs ersichtlich sein</t>
-  </si>
-  <si>
-    <t>der Benutzer soll seinen Post nicht hochladen können, wenn der Post zu lang ist</t>
-  </si>
-  <si>
-    <t>Als Benutzer soll man die Möglichkeit haben das Layout der Seite zu ändern</t>
   </si>
 </sst>
 </file>
@@ -416,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -431,19 +422,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -732,42 +726,42 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="8" t="s">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
       <c r="L3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
       <c r="L4" t="s">
         <v>3</v>
       </c>
@@ -775,19 +769,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
       <c r="L5" t="s">
         <v>2</v>
       </c>
@@ -795,41 +789,41 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
       <c r="L6" t="s">
         <v>4</v>
       </c>
       <c r="M6" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
       <c r="L7" t="s">
         <v>5</v>
       </c>
@@ -837,19 +831,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
       <c r="L8" t="s">
         <v>6</v>
       </c>
@@ -857,19 +851,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="D9" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
       <c r="L9" t="s">
         <v>7</v>
       </c>
@@ -877,12 +871,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L10" t="s">
         <v>8</v>
@@ -891,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L11" t="s">
         <v>9</v>
       </c>
@@ -899,7 +893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L12" t="s">
         <v>10</v>
       </c>
@@ -907,7 +901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L13" t="s">
         <v>11</v>
       </c>
@@ -915,7 +909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L14" t="s">
         <v>12</v>
       </c>
@@ -925,13 +919,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="C3:J3"/>
     <mergeCell ref="D6:J6"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="C3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -946,9 +940,9 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
@@ -960,38 +954,38 @@
       <c r="I3" s="4"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>50</v>
       </c>
@@ -1005,48 +999,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
   <dimension ref="B4:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="10" max="10" width="40" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" customWidth="1"/>
-    <col min="13" max="13" width="20.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C6" s="8" t="s">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
       <c r="K6" t="s">
         <v>32</v>
       </c>
@@ -1057,21 +1051,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>27</v>
       </c>
@@ -1088,7 +1082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>30</v>
       </c>
@@ -1105,7 +1099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>36</v>
       </c>
@@ -1122,12 +1116,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K11" t="s">
         <v>33</v>
@@ -1139,24 +1133,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>27</v>
       </c>
@@ -1173,7 +1167,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>30</v>
       </c>
@@ -1190,7 +1184,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>42</v>
       </c>
@@ -1207,7 +1201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>44</v>
       </c>
@@ -1224,7 +1218,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>46</v>
       </c>
@@ -1241,7 +1235,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>48</v>
       </c>
@@ -1258,37 +1252,36 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
       <c r="K20" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="L20" s="2">
+        <v>43522</v>
+      </c>
+      <c r="M20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
       <c r="K21" t="s">
         <v>34</v>
       </c>
@@ -1299,12 +1292,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" t="s">
         <v>75</v>
-      </c>
-      <c r="D22" t="s">
-        <v>76</v>
       </c>
       <c r="K22" t="s">
         <v>34</v>
@@ -1316,69 +1309,52 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="K23" t="s">
         <v>34</v>
       </c>
       <c r="L23" s="2">
-        <v>43522</v>
+        <v>43543</v>
       </c>
       <c r="M23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K24" t="s">
-        <v>34</v>
-      </c>
-      <c r="L24" s="2">
-        <v>43543</v>
-      </c>
-      <c r="M24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
         <v>57</v>
-      </c>
-      <c r="D27" t="s">
-        <v>59</v>
       </c>
       <c r="K27" t="s">
         <v>34</v>
@@ -1390,24 +1366,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
         <v>58</v>
       </c>
-      <c r="D28" t="s">
-        <v>60</v>
-      </c>
       <c r="K28" t="s">
         <v>34</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>102</v>
+      <c r="L28" s="2">
+        <v>43522</v>
       </c>
       <c r="M28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -1415,12 +1391,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K32" t="s">
         <v>34</v>
@@ -1432,12 +1408,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K33" t="s">
         <v>34</v>
@@ -1449,12 +1425,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K34" t="s">
         <v>33</v>
@@ -1466,12 +1442,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K35" t="s">
         <v>34</v>
@@ -1483,12 +1459,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>46</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K36" t="s">
         <v>33</v>
@@ -1500,12 +1476,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K37" t="s">
         <v>34</v>
@@ -1517,12 +1493,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K38" t="s">
         <v>34</v>
@@ -1534,12 +1510,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K39" t="s">
         <v>34</v>
@@ -1551,12 +1527,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K40" t="s">
         <v>34</v>
@@ -1568,12 +1544,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K41" t="s">
         <v>34</v>
@@ -1585,12 +1561,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K42" t="s">
         <v>34</v>
@@ -1602,12 +1578,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K43" t="s">
         <v>34</v>
@@ -1619,12 +1595,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D44" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K44" t="s">
         <v>34</v>
@@ -1636,10 +1612,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>6</v>
       </c>
@@ -1647,12 +1623,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K47" t="s">
         <v>34</v>
@@ -1664,12 +1640,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K48" t="s">
         <v>34</v>
@@ -1681,12 +1657,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>42</v>
       </c>
       <c r="D49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K49" t="s">
         <v>34</v>
@@ -1698,7 +1674,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>7</v>
       </c>
@@ -1706,12 +1682,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>27</v>
       </c>
       <c r="D52" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K52" t="s">
         <v>34</v>
@@ -1723,12 +1699,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D53" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K53" t="s">
         <v>34</v>
@@ -1740,12 +1716,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>36</v>
       </c>
       <c r="D54" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K54" t="s">
         <v>34</v>
@@ -1757,12 +1733,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K55" t="s">
         <v>34</v>
@@ -1774,7 +1750,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>8</v>
       </c>
@@ -1782,19 +1758,19 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C59" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C59" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>27</v>
       </c>
       <c r="D60" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K60" t="s">
         <v>33</v>
@@ -1806,12 +1782,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K61" t="s">
         <v>33</v>
@@ -1823,12 +1799,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>36</v>
       </c>
       <c r="D62" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K62" t="s">
         <v>33</v>
@@ -1840,12 +1816,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>44</v>
       </c>
       <c r="D63" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K63" t="s">
         <v>33</v>
@@ -1857,29 +1833,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>46</v>
       </c>
       <c r="D64" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="K64" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L64" s="2">
         <v>43564</v>
       </c>
       <c r="M64" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="65" spans="3:13" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D65" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K65" t="s">
         <v>34</v>
@@ -1891,72 +1867,77 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>51</v>
       </c>
       <c r="D66" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K66" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L66" s="2">
         <v>43550</v>
       </c>
-    </row>
-    <row r="67" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="M66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D67" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L67" s="2">
         <v>43550</v>
       </c>
-    </row>
-    <row r="69" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-    </row>
-    <row r="70" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="M67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+    </row>
+    <row r="70" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L72" s="2"/>
     </row>
-    <row r="76" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C76" s="11"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-    </row>
-    <row r="77" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C76" s="12"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+    </row>
+    <row r="77" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L78" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="L25:R25"/>
+    <mergeCell ref="C13:I13"/>
     <mergeCell ref="C59:E59"/>
     <mergeCell ref="C76:E76"/>
     <mergeCell ref="C69:E69"/>
     <mergeCell ref="C26:I26"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="L25:R25"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="D20:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploading/Änderung des Profilbildes erneut hinzugefügt
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C9632F-1352-4A8E-9A85-DE6EF9D735DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE1C6C5-658C-4B98-8CBF-AA5C79281D38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Userstories" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="106">
   <si>
     <t>Userstories</t>
   </si>
@@ -339,19 +339,7 @@
     <t>Als Benutzer soll man die Möglichkeit haben das Layout der Seite zu ändern</t>
   </si>
   <si>
-    <t xml:space="preserve">9. Task </t>
-  </si>
-  <si>
-    <t>Man soll über einen Button Freunde hinzufügen können</t>
-  </si>
-  <si>
     <t>in Arbeit</t>
-  </si>
-  <si>
-    <t>Man soll nur die Feeds seiner Freunde sehen (der neueste Feed zuerst)</t>
-  </si>
-  <si>
-    <t>Projektabgabe am 26.04.2019!!!!!</t>
   </si>
 </sst>
 </file>
@@ -419,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -450,11 +438,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -743,13 +726,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
@@ -766,7 +749,7 @@
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -786,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -806,7 +789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -828,7 +811,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -848,7 +831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -868,7 +851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -888,7 +871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -902,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L11" t="s">
         <v>9</v>
       </c>
@@ -910,7 +893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L12" t="s">
         <v>10</v>
       </c>
@@ -918,7 +901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L13" t="s">
         <v>11</v>
       </c>
@@ -926,7 +909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L14" t="s">
         <v>12</v>
       </c>
@@ -957,9 +940,9 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
@@ -971,38 +954,38 @@
       <c r="I3" s="4"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>50</v>
       </c>
@@ -1016,20 +999,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224001FC-4B11-4D41-A1CC-81545EF3336A}">
   <dimension ref="B4:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E71" sqref="D71:I72"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="10" max="10" width="40" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" customWidth="1"/>
-    <col min="13" max="13" width="20.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -1039,7 +1022,7 @@
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -1048,7 +1031,7 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C6" s="11" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1051,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1082,7 +1065,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>27</v>
       </c>
@@ -1099,7 +1082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>30</v>
       </c>
@@ -1116,7 +1099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>36</v>
       </c>
@@ -1133,7 +1116,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>44</v>
       </c>
@@ -1150,10 +1133,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -1167,7 +1150,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>27</v>
       </c>
@@ -1184,7 +1167,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>30</v>
       </c>
@@ -1201,7 +1184,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>42</v>
       </c>
@@ -1218,7 +1201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>44</v>
       </c>
@@ -1235,7 +1218,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>46</v>
       </c>
@@ -1252,7 +1235,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>48</v>
       </c>
@@ -1269,7 +1252,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>69</v>
       </c>
@@ -1292,7 +1275,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>72</v>
       </c>
@@ -1309,7 +1292,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>74</v>
       </c>
@@ -1326,7 +1309,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>81</v>
       </c>
@@ -1343,7 +1326,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
@@ -1352,7 +1335,7 @@
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -1366,7 +1349,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>55</v>
       </c>
@@ -1383,7 +1366,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>56</v>
       </c>
@@ -1400,7 +1383,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -1408,7 +1391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>27</v>
       </c>
@@ -1425,7 +1408,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>30</v>
       </c>
@@ -1442,7 +1425,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>61</v>
       </c>
@@ -1459,7 +1442,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>63</v>
       </c>
@@ -1476,7 +1459,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>46</v>
       </c>
@@ -1493,7 +1476,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>65</v>
       </c>
@@ -1510,7 +1493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>51</v>
       </c>
@@ -1527,7 +1510,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>69</v>
       </c>
@@ -1544,7 +1527,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>72</v>
       </c>
@@ -1561,7 +1544,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>80</v>
       </c>
@@ -1578,7 +1561,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>81</v>
       </c>
@@ -1595,7 +1578,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>94</v>
       </c>
@@ -1612,7 +1595,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>95</v>
       </c>
@@ -1629,10 +1612,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>6</v>
       </c>
@@ -1640,7 +1623,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>27</v>
       </c>
@@ -1657,7 +1640,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>76</v>
       </c>
@@ -1674,7 +1657,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>42</v>
       </c>
@@ -1691,7 +1674,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>7</v>
       </c>
@@ -1699,7 +1682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>27</v>
       </c>
@@ -1716,7 +1699,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>76</v>
       </c>
@@ -1733,7 +1716,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>36</v>
       </c>
@@ -1750,7 +1733,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>100</v>
       </c>
@@ -1767,7 +1750,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>8</v>
       </c>
@@ -1775,14 +1758,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C59" s="12" t="s">
         <v>92</v>
       </c>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>27</v>
       </c>
@@ -1799,7 +1782,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>30</v>
       </c>
@@ -1816,7 +1799,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>36</v>
       </c>
@@ -1833,7 +1816,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>44</v>
       </c>
@@ -1850,7 +1833,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>46</v>
       </c>
@@ -1867,7 +1850,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>65</v>
       </c>
@@ -1884,7 +1867,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>51</v>
       </c>
@@ -1895,13 +1878,13 @@
         <v>33</v>
       </c>
       <c r="L66" s="2">
-        <v>43581</v>
+        <v>43550</v>
       </c>
       <c r="M66" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="67" spans="3:13" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>69</v>
       </c>
@@ -1912,73 +1895,35 @@
         <v>33</v>
       </c>
       <c r="L67" s="2">
-        <v>43581</v>
+        <v>43550</v>
       </c>
       <c r="M67" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="68" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C68" t="s">
         <v>105</v>
       </c>
-      <c r="D68" t="s">
-        <v>106</v>
-      </c>
-      <c r="K68" t="s">
-        <v>34</v>
-      </c>
-      <c r="L68" s="2">
-        <v>43581</v>
-      </c>
-      <c r="M68" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="69" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C69" t="s">
-        <v>80</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="E69" s="14"/>
-      <c r="K69" t="s">
-        <v>34</v>
-      </c>
-      <c r="L69" s="2">
-        <v>43581</v>
-      </c>
-      <c r="M69" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="70" spans="3:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+    </row>
+    <row r="70" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="D72" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="16"/>
-      <c r="H72" s="16"/>
-      <c r="I72" s="16"/>
+    <row r="72" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L72" s="2"/>
     </row>
-    <row r="76" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C76" s="12"/>
       <c r="D76" s="10"/>
       <c r="E76" s="10"/>
     </row>
-    <row r="77" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:13" x14ac:dyDescent="0.25">
       <c r="L78" s="2"/>
     </row>
   </sheetData>
@@ -1987,9 +1932,9 @@
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="L25:R25"/>
     <mergeCell ref="C13:I13"/>
-    <mergeCell ref="D72:I72"/>
     <mergeCell ref="C59:E59"/>
     <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C69:E69"/>
     <mergeCell ref="C26:I26"/>
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C7:I7"/>

</xml_diff>